<commit_message>
skill timeline event system, input system
</commit_message>
<xml_diff>
--- a/Unity/Assets/Config/Excel/SkillConfig.xlsx
+++ b/Unity/Assets/Config/Excel/SkillConfig.xlsx
@@ -5,23 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nova\Legends-Of-Heroes\Unity\Assets\Config\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sky\Legends-Of-Heroes\Unity\Assets\Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813F8909-EEFF-487C-BFF4-127A1D3F3BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570C93FE-1E51-427E-8A94-E0DA912C0140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="1935" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22875" yWindow="1965" windowWidth="21720" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Skill" sheetId="1" r:id="rId1"/>
     <sheet name="#说明" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" calcOnSave="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -143,9 +143,6 @@
     <t>持续时长0（一帧）</t>
   </si>
   <si>
-    <t>持续时长毫秒</t>
-  </si>
-  <si>
     <t>参数4</t>
   </si>
   <si>
@@ -192,6 +189,15 @@
   </si>
   <si>
     <t>0,1,5000</t>
+  </si>
+  <si>
+    <t>参数0</t>
+  </si>
+  <si>
+    <t>技能抽象类型</t>
+  </si>
+  <si>
+    <t>AbstractType</t>
   </si>
 </sst>
 </file>
@@ -661,330 +667,364 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:J17"/>
+  <dimension ref="C2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="2" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="2"/>
+    <col min="3" max="5" width="12.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="28.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" style="5" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:10">
+    <row r="2" spans="3:11">
       <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="3:10">
+    <row r="3" spans="3:11">
       <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:11">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="I4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="K4" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="3:10">
+    <row r="5" spans="3:11">
       <c r="C5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="E5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="3:10" s="1" customFormat="1">
+    <row r="6" spans="3:11" s="1" customFormat="1">
       <c r="C6" s="1">
         <v>1001</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>1000</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>3000</v>
       </c>
-      <c r="J6" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" s="1" customFormat="1">
+      <c r="K6" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" s="1" customFormat="1">
       <c r="C7" s="1">
         <v>1001</v>
       </c>
       <c r="D7" s="1">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>1000</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>3000</v>
       </c>
-      <c r="J7" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" s="1" customFormat="1">
+      <c r="K7" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" s="1" customFormat="1">
       <c r="C8" s="1">
         <v>1001</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>1000</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>3000</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" s="1" customFormat="1">
+      <c r="K8" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" s="1" customFormat="1">
       <c r="C9" s="1">
         <v>1001</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>1000</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>3000</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10">
+      <c r="K9" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11">
       <c r="C10" s="1">
         <v>1002</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1">
         <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>1000</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>2000</v>
       </c>
-      <c r="J10" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10">
+      <c r="K10" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11">
       <c r="C11" s="1">
         <v>1002</v>
       </c>
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>1000</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>2000</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="3:10">
+      <c r="K11" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
       <c r="C12" s="1">
         <v>1002</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="1">
         <v>2</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>1000</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>2000</v>
       </c>
-      <c r="J12" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="3:10">
+      <c r="K12" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11">
       <c r="C13" s="1">
         <v>1002</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="1">
         <v>2</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>1000</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>2000</v>
       </c>
-      <c r="J13" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="3:10">
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="3:10">
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="10:10">
-      <c r="J17" s="7"/>
+      <c r="K13" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11">
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="3:11">
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="3:11">
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="11:11">
+      <c r="K17" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -998,24 +1038,24 @@
   <dimension ref="B4:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="17.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:10">
       <c r="B4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -1026,16 +1066,19 @@
         <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
-        <v>41</v>
+      <c r="G5" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -1043,35 +1086,32 @@
         <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
         <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="F8" t="s">
-        <v>40</v>
-      </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>